<commit_message>
added script for inserting data
</commit_message>
<xml_diff>
--- a/generate_data.xlsx
+++ b/generate_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Desktop\UNI\4-CUARTO\4-1-WEB APPS\PROJECT\web_apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4886813-05AB-496D-B4CA-163AE6653B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF51047-D580-426D-A227-6D2CCFA04D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{5C59C44A-8F3E-4693-A319-E23D350C6F1B}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{5C59C44A-8F3E-4693-A319-E23D350C6F1B}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="160">
   <si>
     <t>email</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -601,11 +604,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +732,7 @@
     <tableColumn id="1" xr3:uid="{25402337-F88B-44C3-A94F-EDAB5632B376}" uniqueName="1" name="recipe_id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{51DFE866-9B75-4059-9537-62B901478E15}" uniqueName="2" name="ingredient_id" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{D262C8F5-F0DF-48FF-9DCE-8F48B45A58D0}" uniqueName="3" name="quantity" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{FDA52648-3863-4A76-9DEE-F24F8647B0FB}" uniqueName="4" name="unit_of_measurement" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{FDA52648-3863-4A76-9DEE-F24F8647B0FB}" uniqueName="4" name="unit_of_measurement" queryTableFieldId="4" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -743,7 +744,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{38D9B0F0-311B-42DE-B465-CCA44F7C3F38}" uniqueName="1" name="recipe_id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{3352D0F1-2C8F-4BA4-B5BD-9C3B6F51183E}" uniqueName="2" name="sequence_number" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{01832824-70E9-48D3-9143-5D1F6550074C}" uniqueName="3" name="description" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{01832824-70E9-48D3-9143-5D1F6550074C}" uniqueName="3" name="description" queryTableFieldId="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1069,37 +1070,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558F7E67-AC62-44E2-B8E5-83E24A0FCE82}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="str">
+      <c r="B2" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT(D2,"@test.es")</f>
         <v>test1@test.es</v>
       </c>
@@ -1109,12 +1113,16 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="str">
+        <f>D2</f>
+        <v>test1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="str">
+      <c r="B3" t="str">
         <f t="shared" ref="B3:B10" si="0" xml:space="preserve"> _xlfn.CONCAT(D3,"@test.es")</f>
         <v>test2@test.es</v>
       </c>
@@ -1124,12 +1132,16 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E11" si="1">D3</f>
+        <v>test2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="str">
+      <c r="B4" t="str">
         <f t="shared" si="0"/>
         <v>test3@test.es</v>
       </c>
@@ -1139,12 +1151,16 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>test3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="str">
+      <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>test4@test.es</v>
       </c>
@@ -1154,12 +1170,16 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>test4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="str">
+      <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>test5@test.es</v>
       </c>
@@ -1169,12 +1189,16 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>test5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="str">
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>test6@test.es</v>
       </c>
@@ -1184,12 +1208,16 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>test6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="str">
+      <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>test7@test.es</v>
       </c>
@@ -1199,12 +1227,16 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>test7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="str">
+      <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>test8@test.es</v>
       </c>
@@ -1214,12 +1246,16 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>test8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="str">
+      <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>test9@test.es</v>
       </c>
@@ -1229,12 +1265,16 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>test9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="str">
+      <c r="B11" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT(D11,"@test.es")</f>
         <v>test10@test.es</v>
       </c>
@@ -1243,6 +1283,10 @@
       </c>
       <c r="D11" t="s">
         <v>21</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>test10</v>
       </c>
     </row>
   </sheetData>
@@ -1301,10 +1345,10 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
       <c r="D2">
@@ -1316,10 +1360,10 @@
       <c r="F2">
         <v>83</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1327,10 +1371,10 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>48</v>
       </c>
       <c r="D3">
@@ -1342,10 +1386,10 @@
       <c r="F3">
         <v>18</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1353,10 +1397,10 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>50</v>
       </c>
       <c r="D4">
@@ -1368,10 +1412,10 @@
       <c r="F4">
         <v>25</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1379,10 +1423,10 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5">
@@ -1394,10 +1438,10 @@
       <c r="F5">
         <v>46</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1405,10 +1449,10 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>55</v>
       </c>
       <c r="D6">
@@ -1420,10 +1464,10 @@
       <c r="F6">
         <v>38</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1431,10 +1475,10 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
       <c r="D7">
@@ -1446,10 +1490,10 @@
       <c r="F7">
         <v>84</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1457,10 +1501,10 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>59</v>
       </c>
       <c r="D8">
@@ -1472,10 +1516,10 @@
       <c r="F8">
         <v>16</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1483,10 +1527,10 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>61</v>
       </c>
       <c r="D9">
@@ -1498,10 +1542,10 @@
       <c r="F9">
         <v>112</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1509,10 +1553,10 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>64</v>
       </c>
       <c r="D10">
@@ -1524,10 +1568,10 @@
       <c r="F10">
         <v>29</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1535,10 +1579,10 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>66</v>
       </c>
       <c r="D11">
@@ -1550,10 +1594,10 @@
       <c r="F11">
         <v>17</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1561,10 +1605,10 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>69</v>
       </c>
       <c r="D12">
@@ -1576,10 +1620,10 @@
       <c r="F12">
         <v>27</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1587,10 +1631,10 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>61</v>
       </c>
       <c r="D13">
@@ -1602,10 +1646,10 @@
       <c r="F13">
         <v>27</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1613,10 +1657,10 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>52</v>
       </c>
       <c r="D14">
@@ -1628,10 +1672,10 @@
       <c r="F14">
         <v>58</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1639,10 +1683,10 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>74</v>
       </c>
       <c r="D15">
@@ -1654,10 +1698,10 @@
       <c r="F15">
         <v>44</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1665,10 +1709,10 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>76</v>
       </c>
       <c r="D16">
@@ -1680,10 +1724,10 @@
       <c r="F16">
         <v>55</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1691,10 +1735,10 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>79</v>
       </c>
       <c r="D17">
@@ -1706,10 +1750,10 @@
       <c r="F17">
         <v>41</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1717,10 +1761,10 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>81</v>
       </c>
       <c r="D18">
@@ -1732,10 +1776,10 @@
       <c r="F18">
         <v>30</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1743,10 +1787,10 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>52</v>
       </c>
       <c r="D19">
@@ -1758,10 +1802,10 @@
       <c r="F19">
         <v>29</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1769,10 +1813,10 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>84</v>
       </c>
       <c r="D20">
@@ -1784,10 +1828,10 @@
       <c r="F20">
         <v>57</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1795,10 +1839,10 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>64</v>
       </c>
       <c r="D21">
@@ -1810,10 +1854,10 @@
       <c r="F21">
         <v>76</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1821,10 +1865,10 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>86</v>
       </c>
       <c r="D22">
@@ -1836,10 +1880,10 @@
       <c r="F22">
         <v>60</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1847,10 +1891,10 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>88</v>
       </c>
       <c r="D23">
@@ -1862,10 +1906,10 @@
       <c r="F23">
         <v>111</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1873,10 +1917,10 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>88</v>
       </c>
       <c r="D24">
@@ -1888,10 +1932,10 @@
       <c r="F24">
         <v>49</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1899,10 +1943,10 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>74</v>
       </c>
       <c r="D25">
@@ -1914,10 +1958,10 @@
       <c r="F25">
         <v>64</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1925,10 +1969,10 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>90</v>
       </c>
       <c r="D26">
@@ -1940,10 +1984,10 @@
       <c r="F26">
         <v>55</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2307,7 +2351,7 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2324,7 +2368,7 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2341,7 +2385,7 @@
       <c r="D4">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2358,7 +2402,7 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2375,7 +2419,7 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2392,7 +2436,7 @@
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2409,7 +2453,7 @@
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2426,7 +2470,7 @@
       <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2443,7 +2487,7 @@
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2460,7 +2504,7 @@
       <c r="D11">
         <v>4</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2477,7 +2521,7 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2494,7 +2538,7 @@
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2511,7 +2555,7 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2528,7 +2572,7 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2545,7 +2589,7 @@
       <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2562,7 +2606,7 @@
       <c r="D17">
         <v>2</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2579,7 +2623,7 @@
       <c r="D18">
         <v>5</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2596,7 +2640,7 @@
       <c r="D19">
         <v>3</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2613,7 +2657,7 @@
       <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2630,7 +2674,7 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2647,7 +2691,7 @@
       <c r="D22">
         <v>3</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2664,7 +2708,7 @@
       <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2681,7 +2725,7 @@
       <c r="D24">
         <v>5</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2698,7 +2742,7 @@
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2715,7 +2759,7 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2732,7 +2776,7 @@
       <c r="D27">
         <v>4</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2749,7 +2793,7 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2766,7 +2810,7 @@
       <c r="D29">
         <v>4</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2783,7 +2827,7 @@
       <c r="D30">
         <v>2</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2800,7 +2844,7 @@
       <c r="D31">
         <v>5</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2817,7 +2861,7 @@
       <c r="D32">
         <v>4</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2834,7 +2878,7 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2851,7 +2895,7 @@
       <c r="D34">
         <v>4</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2868,7 +2912,7 @@
       <c r="D35">
         <v>2</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2885,7 +2929,7 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2902,7 +2946,7 @@
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2919,7 +2963,7 @@
       <c r="D38">
         <v>4</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2936,7 +2980,7 @@
       <c r="D39">
         <v>3</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2953,7 +2997,7 @@
       <c r="D40">
         <v>3</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2970,7 +3014,7 @@
       <c r="D41">
         <v>2</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2987,7 +3031,7 @@
       <c r="D42">
         <v>2</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3004,7 +3048,7 @@
       <c r="D43">
         <v>2</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3021,7 +3065,7 @@
       <c r="D44">
         <v>5</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3038,7 +3082,7 @@
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3055,7 +3099,7 @@
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3072,7 +3116,7 @@
       <c r="D47">
         <v>4</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3089,7 +3133,7 @@
       <c r="D48">
         <v>2</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3106,7 +3150,7 @@
       <c r="D49">
         <v>5</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3123,7 +3167,7 @@
       <c r="D50">
         <v>2</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3140,7 +3184,7 @@
       <c r="D51">
         <v>3</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3157,7 +3201,7 @@
       <c r="D52">
         <v>2</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3174,7 +3218,7 @@
       <c r="D53">
         <v>2</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3191,7 +3235,7 @@
       <c r="D54">
         <v>5</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3208,7 +3252,7 @@
       <c r="D55">
         <v>4</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3225,7 +3269,7 @@
       <c r="D56">
         <v>5</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3242,7 +3286,7 @@
       <c r="D57">
         <v>4</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3259,7 +3303,7 @@
       <c r="D58">
         <v>4</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3276,7 +3320,7 @@
       <c r="D59">
         <v>3</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3293,7 +3337,7 @@
       <c r="D60">
         <v>4</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3310,7 +3354,7 @@
       <c r="D61">
         <v>4</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3327,7 +3371,7 @@
       <c r="D62">
         <v>5</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3344,7 +3388,7 @@
       <c r="D63">
         <v>5</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3361,7 +3405,7 @@
       <c r="D64">
         <v>4</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3378,7 +3422,7 @@
       <c r="D65">
         <v>2</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3395,7 +3439,7 @@
       <c r="D66">
         <v>2</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3412,7 +3456,7 @@
       <c r="D67">
         <v>1</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3429,7 +3473,7 @@
       <c r="D68">
         <v>5</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3446,7 +3490,7 @@
       <c r="D69">
         <v>3</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3463,7 +3507,7 @@
       <c r="D70">
         <v>5</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3480,7 +3524,7 @@
       <c r="D71">
         <v>4</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3497,7 +3541,7 @@
       <c r="D72">
         <v>2</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3514,7 +3558,7 @@
       <c r="D73">
         <v>3</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3531,7 +3575,7 @@
       <c r="D74">
         <v>5</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3548,7 +3592,7 @@
       <c r="D75">
         <v>2</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3565,7 +3609,7 @@
       <c r="D76">
         <v>4</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3582,7 +3626,7 @@
       <c r="D77">
         <v>1</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3599,7 +3643,7 @@
       <c r="D78">
         <v>5</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3616,7 +3660,7 @@
       <c r="D79">
         <v>5</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3633,7 +3677,7 @@
       <c r="D80">
         <v>4</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3650,7 +3694,7 @@
       <c r="D81">
         <v>1</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3667,7 +3711,7 @@
       <c r="D82">
         <v>5</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3684,7 +3728,7 @@
       <c r="D83">
         <v>3</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3701,7 +3745,7 @@
       <c r="D84">
         <v>4</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3718,7 +3762,7 @@
       <c r="D85">
         <v>2</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3735,7 +3779,7 @@
       <c r="D86">
         <v>5</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E86" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3752,7 +3796,7 @@
       <c r="D87">
         <v>1</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E87" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3769,7 +3813,7 @@
       <c r="D88">
         <v>4</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3786,7 +3830,7 @@
       <c r="D89">
         <v>1</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3803,7 +3847,7 @@
       <c r="D90">
         <v>1</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3820,7 +3864,7 @@
       <c r="D91">
         <v>4</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3837,7 +3881,7 @@
       <c r="D92">
         <v>5</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3854,7 +3898,7 @@
       <c r="D93">
         <v>4</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3871,7 +3915,7 @@
       <c r="D94">
         <v>3</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E94" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3888,7 +3932,7 @@
       <c r="D95">
         <v>2</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E95" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3905,7 +3949,7 @@
       <c r="D96">
         <v>4</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E96" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3922,7 +3966,7 @@
       <c r="D97">
         <v>1</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E97" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3939,7 +3983,7 @@
       <c r="D98">
         <v>4</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E98" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3956,7 +4000,7 @@
       <c r="D99">
         <v>1</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E99" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3973,7 +4017,7 @@
       <c r="D100">
         <v>4</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E100" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3990,7 +4034,7 @@
       <c r="D101">
         <v>1</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4007,7 +4051,7 @@
       <c r="D102">
         <v>5</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E102" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4024,7 +4068,7 @@
       <c r="D103">
         <v>2</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E103" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4041,7 +4085,7 @@
       <c r="D104">
         <v>1</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E104" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4058,7 +4102,7 @@
       <c r="D105">
         <v>5</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="E105" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4075,7 +4119,7 @@
       <c r="D106">
         <v>1</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E106" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4092,7 +4136,7 @@
       <c r="D107">
         <v>3</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="E107" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4109,7 +4153,7 @@
       <c r="D108">
         <v>1</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E108" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4126,7 +4170,7 @@
       <c r="D109">
         <v>4</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E109" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4143,7 +4187,7 @@
       <c r="D110">
         <v>3</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="E110" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4160,7 +4204,7 @@
       <c r="D111">
         <v>4</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E111" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4177,7 +4221,7 @@
       <c r="D112">
         <v>5</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="E112" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4194,7 +4238,7 @@
       <c r="D113">
         <v>1</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="E113" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4211,7 +4255,7 @@
       <c r="D114">
         <v>3</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="E114" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4228,7 +4272,7 @@
       <c r="D115">
         <v>4</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E115" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4245,7 +4289,7 @@
       <c r="D116">
         <v>1</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="E116" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4262,7 +4306,7 @@
       <c r="D117">
         <v>1</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="E117" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4279,7 +4323,7 @@
       <c r="D118">
         <v>2</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E118" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4296,7 +4340,7 @@
       <c r="D119">
         <v>3</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="E119" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4313,7 +4357,7 @@
       <c r="D120">
         <v>4</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="E120" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4330,7 +4374,7 @@
       <c r="D121">
         <v>5</v>
       </c>
-      <c r="E121" s="1" t="s">
+      <c r="E121" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4347,7 +4391,7 @@
       <c r="D122">
         <v>3</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="E122" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4364,7 +4408,7 @@
       <c r="D123">
         <v>5</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="E123" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4381,7 +4425,7 @@
       <c r="D124">
         <v>1</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="E124" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4398,7 +4442,7 @@
       <c r="D125">
         <v>2</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="E125" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4415,7 +4459,7 @@
       <c r="D126">
         <v>3</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="E126" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4432,7 +4476,7 @@
       <c r="D127">
         <v>4</v>
       </c>
-      <c r="E127" s="1" t="s">
+      <c r="E127" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4449,7 +4493,7 @@
       <c r="D128">
         <v>5</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="E128" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4466,7 +4510,7 @@
       <c r="D129">
         <v>2</v>
       </c>
-      <c r="E129" s="1" t="s">
+      <c r="E129" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4483,7 +4527,7 @@
       <c r="D130">
         <v>4</v>
       </c>
-      <c r="E130" s="1" t="s">
+      <c r="E130" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4500,7 +4544,7 @@
       <c r="D131">
         <v>4</v>
       </c>
-      <c r="E131" s="1" t="s">
+      <c r="E131" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4517,7 +4561,7 @@
       <c r="D132">
         <v>1</v>
       </c>
-      <c r="E132" s="1" t="s">
+      <c r="E132" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4534,7 +4578,7 @@
       <c r="D133">
         <v>2</v>
       </c>
-      <c r="E133" s="1" t="s">
+      <c r="E133" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4551,7 +4595,7 @@
       <c r="D134">
         <v>3</v>
       </c>
-      <c r="E134" s="1" t="s">
+      <c r="E134" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4568,7 +4612,7 @@
       <c r="D135">
         <v>3</v>
       </c>
-      <c r="E135" s="1" t="s">
+      <c r="E135" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4585,7 +4629,7 @@
       <c r="D136">
         <v>3</v>
       </c>
-      <c r="E136" s="1" t="s">
+      <c r="E136" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4602,7 +4646,7 @@
       <c r="D137">
         <v>5</v>
       </c>
-      <c r="E137" s="1" t="s">
+      <c r="E137" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4619,7 +4663,7 @@
       <c r="D138">
         <v>3</v>
       </c>
-      <c r="E138" s="1" t="s">
+      <c r="E138" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4636,7 +4680,7 @@
       <c r="D139">
         <v>1</v>
       </c>
-      <c r="E139" s="1" t="s">
+      <c r="E139" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4653,7 +4697,7 @@
       <c r="D140">
         <v>5</v>
       </c>
-      <c r="E140" s="1" t="s">
+      <c r="E140" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4670,7 +4714,7 @@
       <c r="D141">
         <v>4</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="E141" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4687,7 +4731,7 @@
       <c r="D142">
         <v>1</v>
       </c>
-      <c r="E142" s="1" t="s">
+      <c r="E142" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4704,7 +4748,7 @@
       <c r="D143">
         <v>4</v>
       </c>
-      <c r="E143" s="1" t="s">
+      <c r="E143" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4721,7 +4765,7 @@
       <c r="D144">
         <v>1</v>
       </c>
-      <c r="E144" s="1" t="s">
+      <c r="E144" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4738,7 +4782,7 @@
       <c r="D145">
         <v>3</v>
       </c>
-      <c r="E145" s="1" t="s">
+      <c r="E145" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4755,7 +4799,7 @@
       <c r="D146">
         <v>4</v>
       </c>
-      <c r="E146" s="1" t="s">
+      <c r="E146" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4772,7 +4816,7 @@
       <c r="D147">
         <v>1</v>
       </c>
-      <c r="E147" s="1" t="s">
+      <c r="E147" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4789,7 +4833,7 @@
       <c r="D148">
         <v>2</v>
       </c>
-      <c r="E148" s="1" t="s">
+      <c r="E148" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4806,7 +4850,7 @@
       <c r="D149">
         <v>3</v>
       </c>
-      <c r="E149" s="1" t="s">
+      <c r="E149" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4823,7 +4867,7 @@
       <c r="D150">
         <v>5</v>
       </c>
-      <c r="E150" s="1" t="s">
+      <c r="E150" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4840,7 +4884,7 @@
       <c r="D151">
         <v>1</v>
       </c>
-      <c r="E151" s="1" t="s">
+      <c r="E151" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4857,7 +4901,7 @@
       <c r="D152">
         <v>4</v>
       </c>
-      <c r="E152" s="1" t="s">
+      <c r="E152" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4874,7 +4918,7 @@
       <c r="D153">
         <v>2</v>
       </c>
-      <c r="E153" s="1" t="s">
+      <c r="E153" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4891,7 +4935,7 @@
       <c r="D154">
         <v>1</v>
       </c>
-      <c r="E154" s="1" t="s">
+      <c r="E154" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4908,7 +4952,7 @@
       <c r="D155">
         <v>2</v>
       </c>
-      <c r="E155" s="1" t="s">
+      <c r="E155" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4960,7 +5004,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4974,7 +5018,7 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4988,7 +5032,7 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>140</v>
       </c>
     </row>
@@ -5002,7 +5046,7 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5016,7 +5060,7 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5030,7 +5074,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5044,7 +5088,7 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5058,7 +5102,7 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5072,7 +5116,7 @@
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5086,7 +5130,7 @@
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5100,7 +5144,7 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5114,7 +5158,7 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5128,7 +5172,7 @@
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5142,7 +5186,7 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5156,7 +5200,7 @@
       <c r="C16">
         <v>5</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5170,7 +5214,7 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5184,7 +5228,7 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5198,7 +5242,7 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5212,7 +5256,7 @@
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5226,7 +5270,7 @@
       <c r="C21">
         <v>5</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5240,7 +5284,7 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5254,7 +5298,7 @@
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5268,7 +5312,7 @@
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5282,7 +5326,7 @@
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5296,7 +5340,7 @@
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5310,7 +5354,7 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5324,7 +5368,7 @@
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5338,7 +5382,7 @@
       <c r="C29">
         <v>3</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5352,7 +5396,7 @@
       <c r="C30">
         <v>4</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5366,7 +5410,7 @@
       <c r="C31">
         <v>5</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5380,7 +5424,7 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5394,7 +5438,7 @@
       <c r="C33">
         <v>2</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5408,7 +5452,7 @@
       <c r="C34">
         <v>3</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5422,7 +5466,7 @@
       <c r="C35">
         <v>4</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5436,7 +5480,7 @@
       <c r="C36">
         <v>5</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5450,7 +5494,7 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5464,7 +5508,7 @@
       <c r="C38">
         <v>2</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5478,7 +5522,7 @@
       <c r="C39">
         <v>3</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5492,7 +5536,7 @@
       <c r="C40">
         <v>4</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5506,7 +5550,7 @@
       <c r="C41">
         <v>5</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5520,7 +5564,7 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>138</v>
       </c>
     </row>
@@ -5534,7 +5578,7 @@
       <c r="C43">
         <v>2</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5548,7 +5592,7 @@
       <c r="C44">
         <v>3</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>140</v>
       </c>
     </row>
@@ -5562,7 +5606,7 @@
       <c r="C45">
         <v>4</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5576,7 +5620,7 @@
       <c r="C46">
         <v>5</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5590,7 +5634,7 @@
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5604,7 +5648,7 @@
       <c r="C48">
         <v>2</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5618,7 +5662,7 @@
       <c r="C49">
         <v>3</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5632,7 +5676,7 @@
       <c r="C50">
         <v>4</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5646,7 +5690,7 @@
       <c r="C51">
         <v>5</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5660,7 +5704,7 @@
       <c r="C52">
         <v>1</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5674,7 +5718,7 @@
       <c r="C53">
         <v>2</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5688,7 +5732,7 @@
       <c r="C54">
         <v>3</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5702,7 +5746,7 @@
       <c r="C55">
         <v>4</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5716,7 +5760,7 @@
       <c r="C56">
         <v>5</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5730,7 +5774,7 @@
       <c r="C57">
         <v>1</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5744,7 +5788,7 @@
       <c r="C58">
         <v>2</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5758,7 +5802,7 @@
       <c r="C59">
         <v>3</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5772,7 +5816,7 @@
       <c r="C60">
         <v>4</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5786,7 +5830,7 @@
       <c r="C61">
         <v>5</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5800,7 +5844,7 @@
       <c r="C62">
         <v>1</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5814,7 +5858,7 @@
       <c r="C63">
         <v>2</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5828,7 +5872,7 @@
       <c r="C64">
         <v>3</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5842,7 +5886,7 @@
       <c r="C65">
         <v>4</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5856,7 +5900,7 @@
       <c r="C66">
         <v>5</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5870,7 +5914,7 @@
       <c r="C67">
         <v>1</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5884,7 +5928,7 @@
       <c r="C68">
         <v>2</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5898,7 +5942,7 @@
       <c r="C69">
         <v>3</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5912,7 +5956,7 @@
       <c r="C70">
         <v>4</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5926,7 +5970,7 @@
       <c r="C71">
         <v>5</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5940,7 +5984,7 @@
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>148</v>
       </c>
     </row>
@@ -5954,7 +5998,7 @@
       <c r="C73">
         <v>2</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>149</v>
       </c>
     </row>
@@ -5968,7 +6012,7 @@
       <c r="C74">
         <v>3</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5982,7 +6026,7 @@
       <c r="C75">
         <v>4</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>151</v>
       </c>
     </row>
@@ -5996,7 +6040,7 @@
       <c r="C76">
         <v>5</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6010,7 +6054,7 @@
       <c r="C77">
         <v>1</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6024,7 +6068,7 @@
       <c r="C78">
         <v>2</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6038,7 +6082,7 @@
       <c r="C79">
         <v>3</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6052,7 +6096,7 @@
       <c r="C80">
         <v>4</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" t="s">
         <v>146</v>
       </c>
     </row>
@@ -6066,7 +6110,7 @@
       <c r="C81">
         <v>5</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6080,7 +6124,7 @@
       <c r="C82">
         <v>1</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6094,7 +6138,7 @@
       <c r="C83">
         <v>2</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6108,7 +6152,7 @@
       <c r="C84">
         <v>3</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6122,7 +6166,7 @@
       <c r="C85">
         <v>4</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" t="s">
         <v>146</v>
       </c>
     </row>
@@ -6136,7 +6180,7 @@
       <c r="C86">
         <v>5</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6150,7 +6194,7 @@
       <c r="C87">
         <v>1</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" t="s">
         <v>153</v>
       </c>
     </row>
@@ -6164,7 +6208,7 @@
       <c r="C88">
         <v>2</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" t="s">
         <v>154</v>
       </c>
     </row>
@@ -6178,7 +6222,7 @@
       <c r="C89">
         <v>3</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" t="s">
         <v>155</v>
       </c>
     </row>
@@ -6192,7 +6236,7 @@
       <c r="C90">
         <v>4</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6206,7 +6250,7 @@
       <c r="C91">
         <v>5</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" t="s">
         <v>157</v>
       </c>
     </row>
@@ -6220,7 +6264,7 @@
       <c r="C92">
         <v>1</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6234,7 +6278,7 @@
       <c r="C93">
         <v>2</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6248,7 +6292,7 @@
       <c r="C94">
         <v>3</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6262,7 +6306,7 @@
       <c r="C95">
         <v>4</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" t="s">
         <v>146</v>
       </c>
     </row>
@@ -6276,7 +6320,7 @@
       <c r="C96">
         <v>5</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6290,7 +6334,7 @@
       <c r="C97">
         <v>1</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" t="s">
         <v>138</v>
       </c>
     </row>
@@ -6304,7 +6348,7 @@
       <c r="C98">
         <v>2</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6318,7 +6362,7 @@
       <c r="C99">
         <v>3</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" t="s">
         <v>140</v>
       </c>
     </row>
@@ -6332,7 +6376,7 @@
       <c r="C100">
         <v>4</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" t="s">
         <v>141</v>
       </c>
     </row>
@@ -6346,7 +6390,7 @@
       <c r="C101">
         <v>5</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" t="s">
         <v>142</v>
       </c>
     </row>
@@ -6360,7 +6404,7 @@
       <c r="C102">
         <v>1</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6374,7 +6418,7 @@
       <c r="C103">
         <v>2</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6388,7 +6432,7 @@
       <c r="C104">
         <v>3</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" t="s">
         <v>150</v>
       </c>
     </row>
@@ -6402,7 +6446,7 @@
       <c r="C105">
         <v>4</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6416,7 +6460,7 @@
       <c r="C106">
         <v>5</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6430,7 +6474,7 @@
       <c r="C107">
         <v>1</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6444,7 +6488,7 @@
       <c r="C108">
         <v>2</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6458,7 +6502,7 @@
       <c r="C109">
         <v>3</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6472,7 +6516,7 @@
       <c r="C110">
         <v>4</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" t="s">
         <v>146</v>
       </c>
     </row>
@@ -6486,7 +6530,7 @@
       <c r="C111">
         <v>5</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6500,7 +6544,7 @@
       <c r="C112">
         <v>1</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6514,7 +6558,7 @@
       <c r="C113">
         <v>2</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6528,7 +6572,7 @@
       <c r="C114">
         <v>3</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6542,7 +6586,7 @@
       <c r="C115">
         <v>4</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" t="s">
         <v>146</v>
       </c>
     </row>
@@ -6556,7 +6600,7 @@
       <c r="C116">
         <v>5</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6570,7 +6614,7 @@
       <c r="C117">
         <v>1</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6584,7 +6628,7 @@
       <c r="C118">
         <v>2</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6598,7 +6642,7 @@
       <c r="C119">
         <v>3</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6612,7 +6656,7 @@
       <c r="C120">
         <v>4</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" t="s">
         <v>146</v>
       </c>
     </row>
@@ -6626,7 +6670,7 @@
       <c r="C121">
         <v>5</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6640,7 +6684,7 @@
       <c r="C122">
         <v>1</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6654,7 +6698,7 @@
       <c r="C123">
         <v>2</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6668,7 +6712,7 @@
       <c r="C124">
         <v>3</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D124" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6682,7 +6726,7 @@
       <c r="C125">
         <v>4</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" t="s">
         <v>146</v>
       </c>
     </row>
@@ -6696,7 +6740,7 @@
       <c r="C126">
         <v>5</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" t="s">
         <v>147</v>
       </c>
     </row>
@@ -7130,7 +7174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F8CFEA-8896-4B70-B30E-A6A4F5463252}">
   <dimension ref="A1:D251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+    <sheetView topLeftCell="A189" workbookViewId="0">
       <selection activeCell="H230" sqref="H230"/>
     </sheetView>
   </sheetViews>

</xml_diff>